<commit_message>
pgadmin vs forced queries
</commit_message>
<xml_diff>
--- a/db/db_analysis/results.xlsx
+++ b/db/db_analysis/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9F5B4010-1524-A34E-BE6E-B8C3BCB5149E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107B021C-96BE-E642-BD69-014C7682A285}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="33920" windowHeight="28300"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="33920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="1376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="1383">
   <si>
     <t>86f146bae3bad9a3b6c2ee6949ed512732040f8ac6899ccba3af6796618cb59b</t>
   </si>
@@ -15776,12 +15776,33 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>queries on pgadmin</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>before spike</t>
+  </si>
+  <si>
+    <t>after spike</t>
+  </si>
+  <si>
+    <t>worst</t>
+  </si>
+  <si>
+    <t>pgadmin</t>
+  </si>
+  <si>
+    <t>forced</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -20851,16 +20872,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D685" totalsRowShown="0">
-  <autoFilter ref="A1:D685"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D685" totalsRowShown="0">
+  <autoFilter ref="A1:D685" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A2:C685">
     <sortCondition ref="C1:C685"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="query hash"/>
-    <tableColumn id="2" name="query" dataDxfId="1"/>
-    <tableColumn id="3" name="time"/>
-    <tableColumn id="4" name="normal distribution" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="query hash"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="query" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="time"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="normal distribution" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -21164,11 +21185,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T685"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S42" sqref="S42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -21206,6 +21227,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>8.9624672842753342E-3</v>
       </c>
+      <c r="E2">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="14" customHeight="1">
       <c r="A3" t="s">
@@ -21221,6 +21245,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>9.3254673212593963E-3</v>
       </c>
+      <c r="E3">
+        <v>61</v>
+      </c>
       <c r="L3" t="s">
         <v>1374</v>
       </c>
@@ -21242,6 +21269,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>9.5059467228721956E-3</v>
       </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
       <c r="L4" t="s">
         <v>1375</v>
       </c>
@@ -21263,6 +21293,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>9.8834952826331469E-3</v>
       </c>
+      <c r="E5">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="14" customHeight="1">
       <c r="A6" t="s">
@@ -21278,6 +21311,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>9.9801225057527081E-3</v>
       </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="14" customHeight="1">
       <c r="A7" t="s">
@@ -21293,6 +21329,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.0128392150933103E-2</v>
       </c>
+      <c r="E7">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="14" customHeight="1">
       <c r="A8" t="s">
@@ -21308,6 +21347,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.0406169579422657E-2</v>
       </c>
+      <c r="E8">
+        <v>61</v>
+      </c>
       <c r="L8" t="s">
         <v>1371</v>
       </c>
@@ -21334,6 +21376,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.0633258408740761E-2</v>
       </c>
+      <c r="E9">
+        <v>61</v>
+      </c>
       <c r="L9" t="s">
         <v>1372</v>
       </c>
@@ -22486,6 +22531,9 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.4947757811480522E-2</v>
       </c>
+      <c r="G81" t="s">
+        <v>1376</v>
+      </c>
       <c r="N81">
         <v>15</v>
       </c>
@@ -22508,6 +22556,18 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.5192808887972312E-2</v>
       </c>
+      <c r="G82" t="s">
+        <v>1377</v>
+      </c>
+      <c r="H82" t="s">
+        <v>1378</v>
+      </c>
+      <c r="I82" t="s">
+        <v>1379</v>
+      </c>
+      <c r="J82" t="s">
+        <v>1380</v>
+      </c>
       <c r="N82">
         <v>16</v>
       </c>
@@ -22530,6 +22590,21 @@
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.5209310094894419E-2</v>
       </c>
+      <c r="F83" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G83">
+        <v>66</v>
+      </c>
+      <c r="H83">
+        <v>61</v>
+      </c>
+      <c r="I83">
+        <v>60</v>
+      </c>
+      <c r="J83">
+        <v>63</v>
+      </c>
       <c r="N83">
         <v>17</v>
       </c>
@@ -22551,6 +22626,21 @@
       <c r="D84">
         <f>_xlfn.NORM.DIST(Table2[[#This Row],[time]], $M$8, $M$9, FALSE)</f>
         <v>1.5323985955825483E-2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1382</v>
+      </c>
+      <c r="G84">
+        <v>34</v>
+      </c>
+      <c r="H84">
+        <v>44</v>
+      </c>
+      <c r="I84">
+        <v>66</v>
+      </c>
+      <c r="J84">
+        <v>74</v>
       </c>
       <c r="N84">
         <v>18</v>

</xml_diff>

<commit_message>
changed size of diagrams
</commit_message>
<xml_diff>
--- a/db/db_analysis/results.xlsx
+++ b/db/db_analysis/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107B021C-96BE-E642-BD69-014C7682A285}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759EB324-8F01-D54A-9C16-38F06F3C695F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="33920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="67860" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -20799,15 +20799,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20834,16 +20834,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1035050</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21188,8 +21188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83:J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>